<commit_message>
template set views with new process that accounts for panes
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/code_description.xlsx
+++ b/resources/DatasetTemplate/code_description.xlsx
@@ -724,9 +724,9 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>